<commit_message>
updated CRUD and added presentation to documentation folder
</commit_message>
<xml_diff>
--- a/documentation/CRUD Matrix.xlsx
+++ b/documentation/CRUD Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Web_Programming_Term_Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C719E32-1F32-47E4-A227-03344456E16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA8CB19-1494-4BFB-9BC5-41D629A25BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B03C1F6E-4781-4E69-8986-20BAD31D5DD9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Foods</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>phpMyAdmin</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC14D148-1BC3-46F7-B77A-750F379191CA}">
-  <dimension ref="A3:E11"/>
+  <dimension ref="A3:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,11 +611,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>